<commit_message>
updating html and network list
</commit_message>
<xml_diff>
--- a/tvDataMultipleNetworks.xlsx
+++ b/tvDataMultipleNetworks.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,22 +460,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2:15 AM</t>
+          <t>10:45 AM</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>E!</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Best Lessons Ever</t>
+          <t>American Pie</t>
         </is>
       </c>
     </row>
@@ -487,22 +487,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2:45 AM</t>
+          <t>3:45 PM</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>E!</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Live From the U.S. Open</t>
+          <t>Modern Family</t>
         </is>
       </c>
     </row>
@@ -514,22 +514,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2:15 AM</t>
+          <t>6:45 PM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>VICE</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Live From the U.S. Open</t>
+          <t>Mysteries of the Unknown</t>
         </is>
       </c>
     </row>
@@ -541,22 +541,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2:45 AM</t>
+          <t>7:15 PM</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>VICE</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Live From the U.S. Open</t>
+          <t>Mysteries of the Unknown</t>
         </is>
       </c>
     </row>
@@ -568,22 +568,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2:15 AM</t>
+          <t>7:45 PM</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>VICE</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023 U.S. Open Golf Championship</t>
+          <t>Mysteries of the Unknown</t>
         </is>
       </c>
     </row>
@@ -595,22 +595,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2:45 AM</t>
+          <t>1:45 PM</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023 U.S. Open Golf Championship</t>
+          <t>Tyler Perry’s A Madea Christmas</t>
         </is>
       </c>
     </row>
@@ -622,22 +622,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>9:15 AM</t>
+          <t>3:45 PM</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Live From the U.S. Open</t>
+          <t>Tyler Perry’s House of Payne</t>
         </is>
       </c>
     </row>
@@ -649,22 +649,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10:15 PM</t>
+          <t>4:45 PM</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>LPGA Tour Golf</t>
+          <t>Tyler Perry’s House of Payne</t>
         </is>
       </c>
     </row>
@@ -676,22 +676,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2:45 AM</t>
+          <t>7:18 PM</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2023 U.S. Open Golf Championship</t>
+          <t>Tyler Perry’s House of Payne</t>
         </is>
       </c>
     </row>
@@ -703,22 +703,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2:15 PM</t>
+          <t>1:45 PM</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>School of Golf</t>
+          <t>Lethal Weapon</t>
         </is>
       </c>
     </row>
@@ -730,22 +730,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10:15 PM</t>
+          <t>2:45 PM</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Live From the U.S. Open</t>
+          <t>Lethal Weapon</t>
         </is>
       </c>
     </row>
@@ -757,22 +757,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2:15 AM</t>
+          <t>5:45 PM</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023 U.S. Open Golf Championship</t>
+          <t>Lethal Weapon 2</t>
         </is>
       </c>
     </row>
@@ -784,22 +784,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2:45 AM</t>
+          <t>3:45 PM</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>GOLF</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023 U.S. Open Golf Championship</t>
+          <t>Tyler Perry’s Madea’s Witness Protection</t>
         </is>
       </c>
     </row>
@@ -811,22 +811,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>7:23 PM</t>
+          <t>3:45 PM</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>VH1</t>
+          <t>BET</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Black Ink Crew</t>
+          <t>All About the Benjamins</t>
         </is>
       </c>
     </row>
@@ -838,22 +838,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6:23 PM</t>
+          <t>8:15 PM</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>VH1</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>What Men Want</t>
+          <t>The Path to Pebble – Inside the 2023 U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -865,22 +865,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>6:23 PM</t>
+          <t>8:45 PM</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>VH1</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Titanic</t>
+          <t>The Path to Pebble – Inside the 2023 U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -892,22 +892,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7:23 PM</t>
+          <t>9:15 PM</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>VH1</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Django Unchained</t>
+          <t>Live From the U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -919,22 +919,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6:23 PM</t>
+          <t>9:45 PM</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>VH1</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>The Neighborhood</t>
+          <t>Live From the U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -946,22 +946,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>9:55 PM</t>
+          <t>10:15 PM</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Law &amp; Order</t>
+          <t>Live From the U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -973,22 +973,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>11:55 PM</t>
+          <t>10:45 PM</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Happy Valley</t>
+          <t>Live From the U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -1000,22 +1000,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>9:15 PM</t>
+          <t>11:15 PM</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Bones</t>
+          <t>Live From the U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -1027,22 +1027,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>10:40 PM</t>
+          <t>2:15 AM</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Bones</t>
+          <t>Live From the U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -1054,22 +1054,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>11:15 PM</t>
+          <t>2:45 AM</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Bones</t>
+          <t>Live From the U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -1081,22 +1081,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>9:15 PM</t>
+          <t>8:15 PM</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Bones</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1108,22 +1108,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>11:40 PM</t>
+          <t>8:45 PM</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Bones</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1135,22 +1135,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10:55 PM</t>
+          <t>9:15 PM</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Salt</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1162,22 +1162,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>11:55 PM</t>
+          <t>9:45 PM</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Salt</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1189,22 +1189,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>6:40 PM</t>
+          <t>10:15 PM</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>The Fifth Element</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1216,22 +1216,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>10:15 PM</t>
+          <t>10:45 PM</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Spaceballs</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1243,22 +1243,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>10:55 PM</t>
+          <t>2:15 AM</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Spaceballs</t>
+          <t>Live From the U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -1270,22 +1270,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>9:55 AM</t>
+          <t>2:45 AM</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Planet Earth</t>
+          <t>Live From the U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -1297,22 +1297,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>10:15 AM</t>
+          <t>8:15 PM</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Planet Earth</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1324,22 +1324,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2:40 PM</t>
+          <t>8:45 PM</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Planet Earth</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1351,22 +1351,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>5:15 PM</t>
+          <t>9:15 PM</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Planet Earth</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1378,22 +1378,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>6:55 PM</t>
+          <t>9:45 PM</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Underworld</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1405,22 +1405,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>7:15 PM</t>
+          <t>10:15 PM</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Underworld</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1432,22 +1432,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>8:15 PM</t>
+          <t>10:45 PM</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Underworld</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1459,22 +1459,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>9:40 PM</t>
+          <t>11:15 PM</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Judge Dredd</t>
+          <t>Live From the U.S. Women’s Open</t>
         </is>
       </c>
     </row>
@@ -1486,22 +1486,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>9:15 AM</t>
+          <t>2:15 AM</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Planet Earth</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1513,22 +1513,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>10:15 AM</t>
+          <t>2:45 AM</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Planet Earth</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1540,22 +1540,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>11:55 AM</t>
+          <t>1:15 PM</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Gods of Egypt</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1567,22 +1567,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>3:15 PM</t>
+          <t>3:45 PM</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Judge Dredd</t>
+          <t>DP World Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1594,22 +1594,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>4:40 PM</t>
+          <t>4:45 PM</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Battle: Los Angeles</t>
+          <t>DP World Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1621,22 +1621,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>9:40 PM</t>
+          <t>5:15 PM</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>BBCA</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>The Walking Dead: Dead City</t>
+          <t>DP World Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1648,22 +1648,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>11:10 AM</t>
+          <t>5:45 PM</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>My 600-Lb. Life</t>
+          <t>DP World Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1675,22 +1675,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>11:35 AM</t>
+          <t>2:15 AM</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>My 600-Lb. Life</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1702,22 +1702,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>2:45 AM</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>GOLF</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Match Me Abroad</t>
+          <t>PGA Tour Golf</t>
         </is>
       </c>
     </row>
@@ -1729,22 +1729,22 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11:50 AM</t>
+          <t>12:15 AM</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>MLBN</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>90 Day Fiancé: Before the 90 Days</t>
+          <t>Quick Pitch</t>
         </is>
       </c>
     </row>
@@ -1756,22 +1756,22 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>12:50 PM</t>
+          <t>1:45 AM</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>MLBN</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>90 Day Fiancé: Before the 90 Days</t>
+          <t>Quick Pitch</t>
         </is>
       </c>
     </row>
@@ -1783,22 +1783,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2:35 AM</t>
+          <t>2:15 AM</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>MLBN</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>90 Day Fiancé</t>
+          <t>Quick Pitch</t>
         </is>
       </c>
     </row>
@@ -1810,22 +1810,22 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11:50 AM</t>
+          <t>12:45 AM</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>MLBN</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Match Me Abroad</t>
+          <t>MLB Baseball</t>
         </is>
       </c>
     </row>
@@ -1837,22 +1837,22 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2:35 AM</t>
+          <t>1:45 AM</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>MLBN</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Doubling Down With the Derricos</t>
+          <t>Quick Pitch</t>
         </is>
       </c>
     </row>
@@ -1864,22 +1864,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>12:15 AM</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>MLBN</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Doubling Down With the Derricos</t>
+          <t>MLB Baseball</t>
         </is>
       </c>
     </row>
@@ -1891,22 +1891,22 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>9:35 AM</t>
+          <t>1:15 AM</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>MLBN</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Long Lost Family</t>
+          <t>Quick Pitch</t>
         </is>
       </c>
     </row>
@@ -1918,22 +1918,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>2:45 AM</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>MLBN</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Dr. Pimple Popper</t>
+          <t>Quick Pitch</t>
         </is>
       </c>
     </row>
@@ -1945,22 +1945,22 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>12:45 AM</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>MLBN</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Hoarding: Buried Alive</t>
+          <t>MLB Baseball</t>
         </is>
       </c>
     </row>
@@ -1972,22 +1972,22 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>6:50 PM</t>
+          <t>1:15 AM</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>MLBN</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Hoarding: Buried Alive</t>
+          <t>Quick Pitch</t>
         </is>
       </c>
     </row>
@@ -1999,22 +1999,22 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>7:10 PM</t>
+          <t>3:29 PM</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>BETHR</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Hoarding: Buried Alive</t>
+          <t>Lethal Legacy</t>
         </is>
       </c>
     </row>
@@ -2026,22 +2026,22 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>7:35 PM</t>
+          <t>5:29 PM</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>BETHR</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Hoarding: Buried Alive</t>
+          <t>Imani</t>
         </is>
       </c>
     </row>
@@ -2053,22 +2053,22 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2:35 AM</t>
+          <t>2:29 AM</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>BETHR</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Match Me Abroad</t>
+          <t>Wayward</t>
         </is>
       </c>
     </row>
@@ -2080,22 +2080,22 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>2:58 AM</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>BETHR</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Match Me Abroad</t>
+          <t>Wayward</t>
         </is>
       </c>
     </row>
@@ -2107,22 +2107,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>6:35 PM</t>
+          <t>9:29 AM</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>BETHR</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>90 Day Fiancé: Before the 90 Days</t>
+          <t>Tyler Perry’s House of Payne</t>
         </is>
       </c>
     </row>
@@ -2134,22 +2134,22 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>7:35 PM</t>
+          <t>9:59 AM</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>BETHR</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>90 Day Fiancé: Before the 90 Days</t>
+          <t>Tyler Perry’s House of Payne</t>
         </is>
       </c>
     </row>
@@ -2161,22 +2161,22 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2:35 AM</t>
+          <t>2:29 AM</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>TLC</t>
+          <t>BETHR</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Dr. Pimple Popper</t>
+          <t>The Fighting Temptations</t>
         </is>
       </c>
     </row>
@@ -2188,22 +2188,22 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2:20 AM</t>
+          <t>9:15 AM</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>NTGEO</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Drain the Oceans</t>
+          <t>Parking Wars</t>
         </is>
       </c>
     </row>
@@ -2215,22 +2215,22 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2:20 AM</t>
+          <t>10:45 AM</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>NTGEO</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Locked Up Abroad</t>
+          <t>Hoarders</t>
         </is>
       </c>
     </row>
@@ -2242,22 +2242,22 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2:20 AM</t>
+          <t>11:45 AM</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>NTGEO</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Life Below Zero</t>
+          <t>Hoarders</t>
         </is>
       </c>
     </row>
@@ -2269,22 +2269,22 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>12:02 AM</t>
+          <t>2:45 AM</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Furious 7</t>
+          <t>Stone Cold Takes on America</t>
         </is>
       </c>
     </row>
@@ -2296,22 +2296,22 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>1:02 AM</t>
+          <t>3:45 PM</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Olympus Has Fallen</t>
+          <t>Den of Thieves</t>
         </is>
       </c>
     </row>
@@ -2323,22 +2323,22 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1:31 AM</t>
+          <t>6:45 PM</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>The Last Witch Hunter</t>
+          <t>White House Down</t>
         </is>
       </c>
     </row>
@@ -2350,22 +2350,22 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2:02 AM</t>
+          <t>2:45 AM</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>The Last Witch Hunter</t>
+          <t>Hoarders</t>
         </is>
       </c>
     </row>
@@ -2377,22 +2377,22 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2:32 AM</t>
+          <t>1:45 PM</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>The Last Witch Hunter</t>
+          <t>I Survived a Crime</t>
         </is>
       </c>
     </row>
@@ -2404,22 +2404,22 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>3:31 PM</t>
+          <t>3:45 PM</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>The Bourne Legacy</t>
+          <t>Court Cam</t>
         </is>
       </c>
     </row>
@@ -2431,22 +2431,22 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>12:02 AM</t>
+          <t>1:45 PM</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>The Hunt</t>
+          <t>Booked: First Day In</t>
         </is>
       </c>
     </row>
@@ -2458,22 +2458,22 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1:02 AM</t>
+          <t>3:45 PM</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>The Hunt</t>
+          <t>60 Days In</t>
         </is>
       </c>
     </row>
@@ -2485,22 +2485,22 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2:02 AM</t>
+          <t>10:45 PM</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Nerve</t>
+          <t>Booked: First Day In</t>
         </is>
       </c>
     </row>
@@ -2512,22 +2512,22 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2:32 AM</t>
+          <t>3:45 PM</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Nerve</t>
+          <t>The First 48</t>
         </is>
       </c>
     </row>
@@ -2539,22 +2539,22 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2:31 PM</t>
+          <t>11:15 PM</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Con Air</t>
+          <t>The First 48</t>
         </is>
       </c>
     </row>
@@ -2566,22 +2566,22 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>12:02 AM</t>
+          <t>9:15 AM</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Independence Day: Resurgence</t>
+          <t>Zombie House Flipping</t>
         </is>
       </c>
     </row>
@@ -2593,22 +2593,22 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>1:02 AM</t>
+          <t>10:45 AM</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Independence Day: Resurgence</t>
+          <t>Zombie House Flipping</t>
         </is>
       </c>
     </row>
@@ -2620,22 +2620,22 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2:02 AM</t>
+          <t>12:45 PM</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>The Boy</t>
+          <t>Deliciously Twisted Classics</t>
         </is>
       </c>
     </row>
@@ -2647,22 +2647,22 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2:32 AM</t>
+          <t>1:15 PM</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>The Boy</t>
+          <t>Neighborhood Wars</t>
         </is>
       </c>
     </row>
@@ -2674,22 +2674,22 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2:02 AM</t>
+          <t>3:45 PM</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Charmed</t>
+          <t>Booked: First Day In</t>
         </is>
       </c>
     </row>
@@ -2701,22 +2701,22 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2:32 AM</t>
+          <t>5:45 PM</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Charmed</t>
+          <t>The First 48</t>
         </is>
       </c>
     </row>
@@ -2728,22 +2728,22 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>1:31 AM</t>
+          <t>6:45 PM</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Mr. &amp; Mrs. Smith</t>
+          <t>The First 48</t>
         </is>
       </c>
     </row>
@@ -2755,22 +2755,22 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>2:02 AM</t>
+          <t>7:15 PM</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Jumanji</t>
+          <t>The First 48</t>
         </is>
       </c>
     </row>
@@ -2782,22 +2782,22 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2:31 AM</t>
+          <t>7:45 PM</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>SYFY</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Jumanji</t>
+          <t>The First 48</t>
         </is>
       </c>
     </row>
@@ -2809,22 +2809,22 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2:20 AM</t>
+          <t>11:15 PM</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>AMC</t>
+          <t>A&amp;E</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Road House</t>
+          <t>The First 48</t>
         </is>
       </c>
     </row>
@@ -2836,22 +2836,22 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>2:20 AM</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>AMC</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Road House</t>
+          <t>Orca vs. Great White</t>
         </is>
       </c>
     </row>
@@ -2863,22 +2863,22 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2:20 AM</t>
+          <t>2:50 AM</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>AMC</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Fear the Walking Dead</t>
+          <t>Orca vs. Great White</t>
         </is>
       </c>
     </row>
@@ -2890,7 +2890,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2900,12 +2900,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>AMC</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>The Perfect Storm</t>
+          <t>World’s Biggest Great White?</t>
         </is>
       </c>
     </row>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2927,12 +2927,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>AMC</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>The Perfect Storm</t>
+          <t>World’s Biggest Great White?</t>
         </is>
       </c>
     </row>
@@ -2944,7 +2944,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2954,12 +2954,12 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>AMC</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>The Walking Dead</t>
+          <t>Camo Sharks</t>
         </is>
       </c>
     </row>
@@ -2971,22 +2971,22 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/05/2023</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>7:45 PM</t>
+          <t>2:50 AM</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>VICE</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Most Expensivest</t>
+          <t>Camo Sharks</t>
         </is>
       </c>
     </row>
@@ -2998,22 +2998,22 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>6:45 PM</t>
+          <t>2:20 AM</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>FYI</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Ice Road Truckers</t>
+          <t>Baby Sharks</t>
         </is>
       </c>
     </row>
@@ -3025,22 +3025,22 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/06/2023</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>7:15 PM</t>
+          <t>2:50 AM</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>FYI</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Ice Road Truckers</t>
+          <t>Baby Sharks</t>
         </is>
       </c>
     </row>
@@ -3052,22 +3052,22 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>6:45 PM</t>
+          <t>2:20 AM</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>E!</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Made of Honor</t>
+          <t>Bull Shark vs. Hammerhead</t>
         </is>
       </c>
     </row>
@@ -3079,22 +3079,22 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>7:15 PM</t>
+          <t>2:50 AM</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>E!</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Mike and Dave Need Wedding Dates</t>
+          <t>Bull Shark vs. Hammerhead</t>
         </is>
       </c>
     </row>
@@ -3106,22 +3106,22 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>2:15 AM</t>
+          <t>6:20 PM</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>When Sharks Attack… And Why</t>
         </is>
       </c>
     </row>
@@ -3133,22 +3133,22 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>2:45 AM</t>
+          <t>2:20 AM</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>Most Extreme Sharks With Steve Backshall</t>
         </is>
       </c>
     </row>
@@ -3160,22 +3160,22 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>2:15 AM</t>
+          <t>2:50 AM</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>NTGEO</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>Most Extreme Sharks With Steve Backshall</t>
         </is>
       </c>
     </row>
@@ -3187,22 +3187,22 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>2:45 AM</t>
+          <t>2:20 AM</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>AMC</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>The Walking Dead: Dead City</t>
         </is>
       </c>
     </row>
@@ -3214,22 +3214,22 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>2:15 AM</t>
+          <t>2:20 AM</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>AMC</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>Fear the Walking Dead</t>
         </is>
       </c>
     </row>
@@ -3241,22 +3241,22 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>2:45 AM</t>
+          <t>2:20 AM</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>AMC</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>Star Trek Into Darkness</t>
         </is>
       </c>
     </row>
@@ -3268,22 +3268,22 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>9:45 AM</t>
+          <t>2:50 AM</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>AMC</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>Star Trek Into Darkness</t>
         </is>
       </c>
     </row>
@@ -3295,22 +3295,22 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>12:15 PM</t>
+          <t>9:35 AM</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3322,22 +3322,22 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>5:15 PM</t>
+          <t>10:35 AM</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>MLB Baseball</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3349,22 +3349,22 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>2:15 AM</t>
+          <t>10:50 AM</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3376,22 +3376,22 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>2:45 AM</t>
+          <t>11:10 AM</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3403,22 +3403,22 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>9:15 AM</t>
+          <t>11:50 AM</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3430,22 +3430,22 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>11:45 AM</t>
+          <t>12:35 PM</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3457,22 +3457,22 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>2:15 AM</t>
+          <t>12:50 PM</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3484,22 +3484,22 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>2:45 AM</t>
+          <t>2:35 PM</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>MLBN</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Quick Pitch</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3511,22 +3511,22 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>9:15 AM</t>
+          <t>2:50 PM</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Parking Wars</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3538,22 +3538,22 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>5:15 PM</t>
+          <t>3:50 PM</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>The First 48</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3565,22 +3565,22 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>5:45 PM</t>
+          <t>7:10 PM</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>The First 48</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3592,22 +3592,22 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>11:15 PM</t>
+          <t>7:50 PM</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>The First 48</t>
+          <t>90 Day Fiancé</t>
         </is>
       </c>
     </row>
@@ -3619,22 +3619,22 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>5:15 PM</t>
+          <t>9:35 AM</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Customer Wars</t>
+          <t>Match Me Abroad</t>
         </is>
       </c>
     </row>
@@ -3646,22 +3646,22 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>6:45 PM</t>
+          <t>11:10 AM</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Customer Wars</t>
+          <t>Match Me Abroad</t>
         </is>
       </c>
     </row>
@@ -3673,22 +3673,22 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>06/13/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>10:45 PM</t>
+          <t>12:35 PM</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Storage Wars</t>
+          <t>Match Me Abroad</t>
         </is>
       </c>
     </row>
@@ -3700,22 +3700,22 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/04/2023</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>12:45 PM</t>
+          <t>3:35 PM</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>The First 48</t>
+          <t>Dr. Pimple Popper</t>
         </is>
       </c>
     </row>
@@ -3727,22 +3727,22 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/07/2023</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>4:45 PM</t>
+          <t>2:50 AM</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Court Cam</t>
+          <t>My Strange Addiction</t>
         </is>
       </c>
     </row>
@@ -3754,22 +3754,22 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>6:45 PM</t>
+          <t>6:35 PM</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Court Cam</t>
+          <t>Extreme Cougar Wives</t>
         </is>
       </c>
     </row>
@@ -3781,22 +3781,22 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>2:45 PM</t>
+          <t>6:50 PM</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Den of Thieves</t>
+          <t>Extreme Cougar Wives</t>
         </is>
       </c>
     </row>
@@ -3808,22 +3808,22 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>9:45 PM</t>
+          <t>7:35 PM</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Exposing Parchman</t>
+          <t>Extreme Cougar Wives</t>
         </is>
       </c>
     </row>
@@ -3835,22 +3835,22 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>5:45 PM</t>
+          <t>7:50 PM</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Booked: First Day In</t>
+          <t>Extreme Cougar Wives</t>
         </is>
       </c>
     </row>
@@ -3862,22 +3862,22 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>7:45 PM</t>
+          <t>12:35 AM</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>WWE’s Most Wanted Treasures</t>
+          <t>90 Day Fiancé: Before the 90 Days</t>
         </is>
       </c>
     </row>
@@ -3889,22 +3889,22 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>11:15 PM</t>
+          <t>2:50 AM</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>A&amp;E</t>
+          <t>TLC</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>WWE’s Most Wanted Treasures</t>
+          <t>Match Me Abroad</t>
         </is>
       </c>
     </row>
@@ -3916,22 +3916,22 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>11:45 AM</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>HGTV</t>
+          <t>PARAM</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>House Hunters International</t>
+          <t>NCIS</t>
         </is>
       </c>
     </row>
@@ -3943,22 +3943,22 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>06/15/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>1:15 PM</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>HGTV</t>
+          <t>PARAM</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>House Hunters</t>
+          <t>John Wick</t>
         </is>
       </c>
     </row>
@@ -3970,22 +3970,22 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>2:45 AM</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>HGTV</t>
+          <t>PARAM</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>House Hunters International</t>
+          <t>John Wick: Chapter 3 — Parabellum</t>
         </is>
       </c>
     </row>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4007,12 +4007,12 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>HGTV</t>
+          <t>TRV</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>100 Day Dream Home</t>
+          <t>Alien Invasion: Hudson Valley</t>
         </is>
       </c>
     </row>
@@ -4024,22 +4024,22 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>06/18/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>2:20 AM</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>HGTV</t>
+          <t>TRV</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>House Hunters</t>
+          <t>Alcatraz: Mysteries at the Museum</t>
         </is>
       </c>
     </row>
@@ -4051,7 +4051,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>06/12/2023</t>
+          <t>07/09/2023</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4066,7 +4066,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Impractical Jokers: Inside Jokes</t>
+          <t>Alcatraz: Mysteries at the Museum</t>
         </is>
       </c>
     </row>
@@ -4078,22 +4078,22 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>06/14/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>2:20 AM</t>
+          <t>6:15 PM</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>TRV</t>
+          <t>BBCA</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Impractical Jokers: Inside Jokes</t>
+          <t>Field of Dreams</t>
         </is>
       </c>
     </row>
@@ -4105,22 +4105,22 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>06/16/2023</t>
+          <t>07/08/2023</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>2:50 AM</t>
+          <t>6:40 PM</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>TRV</t>
+          <t>BBCA</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Impractical Jokers: Inside Jokes</t>
+          <t>Field of Dreams</t>
         </is>
       </c>
     </row>
@@ -4132,22 +4132,22 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>2:28 AM</t>
+          <t>12:02 PM</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>BETHR</t>
+          <t>SYFY</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Angrily Ever After</t>
+          <t>Coneheads</t>
         </is>
       </c>
     </row>
@@ -4159,22 +4159,751 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>06/17/2023</t>
+          <t>07/03/2023</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>2:59 AM</t>
+          <t>2:02 PM</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>BETHR</t>
+          <t>SYFY</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Angrily Ever After</t>
+          <t>The Day the Earth Stood Still</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>07/03/2023</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>2:02 AM</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Back to the Future Part III</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>07/04/2023</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>12:02 PM</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>The Twilight Zone</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>07/04/2023</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>2:02 PM</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>The Twilight Zone</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>07/04/2023</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>2:32 AM</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Kick-Ass</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>07/05/2023</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>10:32 AM</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Midnight in the Switchgrass</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>07/05/2023</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>11:31 AM</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Midnight in the Switchgrass</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>07/05/2023</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>12:31 PM</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Escape Plan</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>07/05/2023</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>1:01 PM</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Escape Plan</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>07/05/2023</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>1:02 AM</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>The Twilight Zone</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>07/05/2023</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>2:02 AM</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>The Twilight Zone</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>07/06/2023</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>11:31 AM</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Escape Plan: The Extractors</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>07/06/2023</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>12:02 PM</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Escape Plan: The Extractors</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>07/06/2023</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>12:31 PM</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Escape Plan: The Extractors</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>07/06/2023</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>2:02 PM</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Blade Runner 2049</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>07/06/2023</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>3:02 PM</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Blade Runner 2049</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>07/06/2023</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>2:02 AM</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Assassin’s Creed</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>10:31 AM</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Killjoys</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>12:02 PM</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Killjoys</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>1:01 PM</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Killjoys</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>3:02 PM</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Killjoys</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>3:31 PM</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Killjoys</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>1:02 AM</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>2 Fast 2 Furious</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>07/07/2023</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>2:02 AM</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Escape Plan: The Extractors</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>07/08/2023</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>2:02 AM</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Escape the Field</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>07/09/2023</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>2:02 AM</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>SYFY</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Bangkok Dangerous</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>07/03/2023</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>2:50 AM</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>HGTV</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>House Hunters International</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>07/09/2023</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>2:50 AM</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>HGTV</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>House Hunters</t>
         </is>
       </c>
     </row>

</xml_diff>